<commit_message>
time sheet and example code
</commit_message>
<xml_diff>
--- a/TImeSheet/TimeSheet.xlsx
+++ b/TImeSheet/TimeSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali\Desktop\School\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ali\Desktop\School\TImeSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>تاریخ</t>
   </si>
@@ -41,9 +41,6 @@
     <t>مجموع</t>
   </si>
   <si>
-    <t>6:45-&gt;7:45 | 8:25-&gt;11:00 |  11:25-&gt;12:35 | 2:00-&gt;3:30 | 3:50-&gt;5:20</t>
-  </si>
-  <si>
     <t>1399/04/11</t>
   </si>
   <si>
@@ -56,38 +53,104 @@
     <t>1399/04/13</t>
   </si>
   <si>
-    <t>7:00-&gt;3:30</t>
-  </si>
-  <si>
-    <t>6:45 -&gt; 7:45 | 9:00-&gt;1:00 |2:00-&gt;5:00</t>
-  </si>
-  <si>
-    <t>7:40-&gt;8:40 |9:00-&gt;10:45 | 11:00-&gt;11:40 | 12:20-&gt;1:00</t>
-  </si>
-  <si>
     <t>1399/04/14</t>
   </si>
   <si>
-    <t>8:00-&gt;4:00</t>
-  </si>
-  <si>
-    <t>9:40-&gt;11:40 |1:00-&gt;2:00| 3:40-&gt;4:40 |4:45-&gt;5:45|6:00-&gt;7:00 | 8:00-&gt;10:00</t>
-  </si>
-  <si>
     <t>1399/04/15</t>
   </si>
   <si>
-    <t>شسزشس</t>
-  </si>
-  <si>
-    <t>7:50-&gt;8:50 | 9:15-&gt;</t>
+    <t>8:00-&gt;16:00</t>
+  </si>
+  <si>
+    <t>7:00-&gt;15:30</t>
+  </si>
+  <si>
+    <t>6:45 -&gt; 7:45 | 9:00-&gt;13:00 |14:00-&gt;17:00</t>
+  </si>
+  <si>
+    <t>7:40-&gt;8:40 |9:00-&gt;10:45 | 11:00-&gt;11:40 | 12:20-&gt;13:00</t>
+  </si>
+  <si>
+    <t>9:40-&gt;11:40 |13:00-&gt;14:00| 15:40-&gt;16:40 |16:45-&gt;17:45|18:00-&gt;19:00 |20:00-&gt;22:00</t>
+  </si>
+  <si>
+    <t>1399/04/16</t>
+  </si>
+  <si>
+    <t>1399/04/17</t>
+  </si>
+  <si>
+    <t>1399/04/18</t>
+  </si>
+  <si>
+    <t>1399/04/19</t>
+  </si>
+  <si>
+    <t>1399/04/20</t>
+  </si>
+  <si>
+    <t>1399/04/21</t>
+  </si>
+  <si>
+    <t>1399/04/22</t>
+  </si>
+  <si>
+    <t>1399/04/23</t>
+  </si>
+  <si>
+    <t>1399/04/24</t>
+  </si>
+  <si>
+    <t>1399/04/25</t>
+  </si>
+  <si>
+    <t>1399/04/26</t>
+  </si>
+  <si>
+    <t>1399/04/27</t>
+  </si>
+  <si>
+    <t>1399/04/28</t>
+  </si>
+  <si>
+    <t>1399/04/29</t>
+  </si>
+  <si>
+    <t>1399/04/30</t>
+  </si>
+  <si>
+    <t>1399/04/31</t>
+  </si>
+  <si>
+    <t>1399/05/01</t>
+  </si>
+  <si>
+    <t>1399/05/02</t>
+  </si>
+  <si>
+    <t>6:45-&gt;7:45 | 8:25-&gt;11:00 |  11:25-&gt;12:35 | 14:00-&gt;15:30 | 15:50-&gt;17:40</t>
+  </si>
+  <si>
+    <t>7:50-&gt;8:50 | 9:15-&gt;10:15 | 11:35-&gt;12:35 | 13:15-&gt;14:15 |14:30-&gt;17:30|</t>
+  </si>
+  <si>
+    <t>7:00-&gt;10:00|11:00-&gt;13:00|14:00-&gt;17:00</t>
+  </si>
+  <si>
+    <t>8:00-&gt;12:00</t>
+  </si>
+  <si>
+    <t>12:00-&gt;16:00</t>
+  </si>
+  <si>
+    <t>18:00-&gt;20:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +184,12 @@
       <charset val="178"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -143,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -154,10 +223,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -439,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,7 +516,7 @@
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="3" max="3" width="99" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -463,7 +529,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -472,26 +538,29 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.3576388888888889</v>
+        <v>34</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
       </c>
       <c r="D4" s="1">
         <v>0</v>
@@ -499,41 +568,289 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.16666666666666666</v>
+        <v>14</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.33333333333333331</v>
+      <c r="D6" s="1">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>17</v>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>